<commit_message>
Se realizan cambios. Version final
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DataPruebas.xlsx
+++ b/src/test/resources/data/DataPruebas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tsoftlatam-my.sharepoint.com/personal/diana_vergara_tsoftglobal_com/Documents/Documentos/Oficina/Capacitacion Selenium/Mineduc_Libros/src/test/resources/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mineduc_Libros\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_AD4D2F04E46CFB4ACB3E20888DD2DB40693EDF2F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E4A7B42-5681-46A8-847F-623B20073931}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A9879B-34ED-4D75-9948-FBD01AE853BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31260" yWindow="2520" windowWidth="16980" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -25,23 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>TituloCPS</t>
   </si>
   <si>
-    <t>CP003</t>
-  </si>
-  <si>
-    <t>CP004</t>
-  </si>
-  <si>
-    <t>CP005</t>
-  </si>
-  <si>
-    <t>CP006</t>
-  </si>
-  <si>
     <t>CP007</t>
   </si>
   <si>
@@ -72,31 +60,58 @@
     <t>CP016</t>
   </si>
   <si>
-    <t>CP002_CreacionCtaSpotify</t>
-  </si>
-  <si>
     <t>Dato1</t>
   </si>
   <si>
     <t>Dato2</t>
   </si>
   <si>
+    <t>13.678.876-0</t>
+  </si>
+  <si>
+    <t>5° Básico</t>
+  </si>
+  <si>
+    <t>11.111.222-M</t>
+  </si>
+  <si>
+    <t>24.304.457-K</t>
+  </si>
+  <si>
+    <t>CP001_ErrorRUTErroneo</t>
+  </si>
+  <si>
+    <t>CP002_ErrorRutInvalido</t>
+  </si>
+  <si>
+    <t>CP003_SinCurso</t>
+  </si>
+  <si>
+    <t>CP004_SinFechaNac</t>
+  </si>
+  <si>
     <t>Dato3</t>
   </si>
   <si>
-    <t>13.678.876-0</t>
-  </si>
-  <si>
-    <t>5° Básico</t>
-  </si>
-  <si>
-    <t>11.111.222-M</t>
-  </si>
-  <si>
-    <t>24.304.457-K</t>
-  </si>
-  <si>
-    <t>CP001_ErrorRUTErroneo</t>
+    <t>Seleccione Fecha de nacimiento</t>
+  </si>
+  <si>
+    <t>Seleccione Curso</t>
+  </si>
+  <si>
+    <t>RUN del estudiante no es válido</t>
+  </si>
+  <si>
+    <t>Según nuestros registros, sus datos no son válidos.</t>
+  </si>
+  <si>
+    <t>.:: Seleccione Curso ::.</t>
+  </si>
+  <si>
+    <t>CP005_IngresoCorrecto</t>
+  </si>
+  <si>
+    <t>CP006_DescargarLibro</t>
   </si>
 </sst>
 </file>
@@ -140,7 +155,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,15 +439,15 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -440,142 +455,147 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="1">
-        <v>41439</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
       <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1">
-        <v>41439</v>
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1">
-        <v>41439</v>
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1">
-        <v>41439</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1">
-        <v>41439</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>